<commit_message>
update project daily log document
</commit_message>
<xml_diff>
--- a/Documents/0 Project Managment/Project Daily Log - 2012.xlsx
+++ b/Documents/0 Project Managment/Project Daily Log - 2012.xlsx
@@ -226,18 +226,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -299,7 +293,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -375,42 +369,55 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -993,10 +1000,10 @@
     </row>
     <row r="7" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1"/>
-      <c r="B7" s="22" t="s">
+      <c r="B7" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="23"/>
+      <c r="C7" s="27"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
     </row>
@@ -1090,7 +1097,7 @@
   <dimension ref="A1:J91"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1417,30 +1424,30 @@
       <c r="J11" s="8"/>
     </row>
     <row r="12" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="24">
+      <c r="A12" s="28">
         <v>11</v>
       </c>
-      <c r="B12" s="25">
+      <c r="B12" s="29">
         <v>41009</v>
       </c>
-      <c r="C12" s="26" t="s">
+      <c r="C12" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="D12" s="27" t="s">
+      <c r="D12" s="31" t="s">
         <v>42</v>
       </c>
-      <c r="E12" s="27" t="s">
+      <c r="E12" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="F12" s="25">
+      <c r="F12" s="29">
         <v>41000</v>
       </c>
-      <c r="G12" s="27"/>
-      <c r="H12" s="27" t="s">
+      <c r="G12" s="31"/>
+      <c r="H12" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="I12" s="24" t="s">
-        <v>15</v>
+      <c r="I12" s="35" t="s">
+        <v>16</v>
       </c>
       <c r="J12" s="8"/>
     </row>
@@ -1556,57 +1563,57 @@
       <c r="J16" s="8"/>
     </row>
     <row r="17" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="28">
+      <c r="A17" s="22">
         <v>16</v>
       </c>
-      <c r="B17" s="29">
+      <c r="B17" s="23">
         <v>41001</v>
       </c>
-      <c r="C17" s="30" t="s">
+      <c r="C17" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="D17" s="31" t="s">
+      <c r="D17" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="E17" s="31" t="s">
+      <c r="E17" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="F17" s="29">
+      <c r="F17" s="23">
         <v>41014</v>
       </c>
-      <c r="G17" s="31"/>
-      <c r="H17" s="31" t="s">
+      <c r="G17" s="25"/>
+      <c r="H17" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="I17" s="28" t="s">
+      <c r="I17" s="22" t="s">
         <v>15</v>
       </c>
       <c r="J17" s="8"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="13">
+      <c r="A18" s="32">
         <v>17</v>
       </c>
-      <c r="B18" s="14">
+      <c r="B18" s="23">
         <v>41009</v>
       </c>
-      <c r="C18" s="19" t="s">
+      <c r="C18" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="33" t="s">
         <v>43</v>
       </c>
-      <c r="E18" s="8" t="s">
+      <c r="E18" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="F18" s="14">
+      <c r="F18" s="23">
         <v>41014</v>
       </c>
-      <c r="G18" s="20"/>
-      <c r="H18" s="8" t="s">
+      <c r="G18" s="25"/>
+      <c r="H18" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="I18" s="13" t="s">
+      <c r="I18" s="32" t="s">
         <v>15</v>
       </c>
       <c r="J18" s="8"/>

</xml_diff>

<commit_message>
update project daily log document and added project plan
</commit_message>
<xml_diff>
--- a/Documents/0 Project Managment/Project Daily Log - 2012.xlsx
+++ b/Documents/0 Project Managment/Project Daily Log - 2012.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="50">
   <si>
     <t>Date of Entry</t>
   </si>
@@ -168,6 +168,9 @@
   </si>
   <si>
     <t>How does Cloud App Studio work?</t>
+  </si>
+  <si>
+    <t>Create "project plan" document</t>
   </si>
 </sst>
 </file>
@@ -1099,8 +1102,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1760,15 +1763,31 @@
       <c r="J23" s="8"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="15"/>
-      <c r="B24" s="9"/>
-      <c r="C24" s="12"/>
-      <c r="D24" s="10"/>
-      <c r="E24" s="10"/>
-      <c r="F24" s="9"/>
+      <c r="A24" s="15">
+        <v>23</v>
+      </c>
+      <c r="B24" s="14">
+        <v>41009</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="E24" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="F24" s="14">
+        <v>41011</v>
+      </c>
       <c r="G24" s="10"/>
-      <c r="H24" s="10"/>
-      <c r="I24" s="11"/>
+      <c r="H24" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="I24" s="11" t="s">
+        <v>16</v>
+      </c>
       <c r="J24" s="8"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
new meeting document. Other updated
</commit_message>
<xml_diff>
--- a/Documents/0 Project Managment/Project Daily Log - 2012.xlsx
+++ b/Documents/0 Project Managment/Project Daily Log - 2012.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="53">
   <si>
     <t>Date of Entry</t>
   </si>
@@ -177,6 +177,9 @@
   </si>
   <si>
     <t>Create "Burndown Chart" document</t>
+  </si>
+  <si>
+    <t>Create "MinutesOfMeeting - w15.3" document</t>
   </si>
 </sst>
 </file>
@@ -305,7 +308,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -432,15 +435,23 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -1120,8 +1131,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26:XFD26"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1557,31 +1568,31 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:10" s="32" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="22">
+    <row r="16" spans="1:10" s="39" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="26">
         <v>15</v>
       </c>
-      <c r="B16" s="23">
+      <c r="B16" s="27">
         <v>41009</v>
       </c>
-      <c r="C16" s="24" t="s">
+      <c r="C16" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="D16" s="32" t="s">
+      <c r="D16" s="39" t="s">
         <v>47</v>
       </c>
-      <c r="E16" s="25" t="s">
+      <c r="E16" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="F16" s="23">
+      <c r="F16" s="27">
         <v>41014</v>
       </c>
-      <c r="G16" s="25"/>
-      <c r="H16" s="25" t="s">
+      <c r="G16" s="29"/>
+      <c r="H16" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="I16" s="22" t="s">
-        <v>15</v>
+      <c r="I16" s="33" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -1834,11 +1845,11 @@
       </c>
       <c r="J25" s="8"/>
     </row>
-    <row r="26" spans="1:10" s="32" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="30">
+    <row r="26" spans="1:10" s="39" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="33">
         <v>25</v>
       </c>
-      <c r="B26" s="23">
+      <c r="B26" s="27">
         <v>41012</v>
       </c>
       <c r="C26" s="36" t="s">
@@ -1850,7 +1861,7 @@
       <c r="E26" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="F26" s="23">
+      <c r="F26" s="27">
         <v>41014</v>
       </c>
       <c r="G26" s="37"/>
@@ -1858,18 +1869,35 @@
         <v>17</v>
       </c>
       <c r="I26" s="38" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B27" s="9"/>
-      <c r="C27" s="12"/>
-      <c r="D27" s="10"/>
-      <c r="E27" s="10"/>
-      <c r="F27" s="9"/>
+      <c r="A27" s="13">
+        <v>26</v>
+      </c>
+      <c r="B27" s="27">
+        <v>41014</v>
+      </c>
+      <c r="C27" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="E27" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="F27" s="27">
+        <v>41015</v>
+      </c>
       <c r="G27" s="10"/>
-      <c r="H27" s="10"/>
-      <c r="I27" s="11"/>
+      <c r="H27" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="I27" s="11" t="s">
+        <v>16</v>
+      </c>
       <c r="J27" s="8"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
update project daily log
</commit_message>
<xml_diff>
--- a/Documents/0 Project Managment/Project Daily Log - 2012.xlsx
+++ b/Documents/0 Project Managment/Project Daily Log - 2012.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="35720" windowHeight="23720" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24240" windowHeight="18240" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Project Data" sheetId="1" r:id="rId1"/>
@@ -238,9 +238,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="yyyy/mm/dd"/>
-    <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -288,18 +287,12 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FFFFFF00"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -331,9 +324,6 @@
   </cellStyleXfs>
   <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -345,14 +335,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -360,27 +350,15 @@
       <alignment vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -388,10 +366,10 @@
       <alignment vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -401,6 +379,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -476,6 +469,11 @@
       <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -848,99 +846,99 @@
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="3" spans="1:5" ht="20">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-    </row>
-    <row r="4" spans="1:5" ht="20">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-    </row>
-    <row r="5" spans="1:5" ht="20">
-      <c r="A5" s="2"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-    </row>
-    <row r="6" spans="1:5" ht="20">
-      <c r="A6" s="2"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-    </row>
-    <row r="7" spans="1:5" ht="30" customHeight="1">
-      <c r="A7" s="2"/>
-      <c r="B7" s="1" t="s">
+    <row r="3" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="A5" s="1"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="A6" s="1"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="1"/>
+      <c r="B7" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="1"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-    </row>
-    <row r="8" spans="1:5" ht="30" customHeight="1">
-      <c r="A8" s="2"/>
-      <c r="B8" s="5" t="s">
+      <c r="C7" s="18"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+    </row>
+    <row r="8" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="1"/>
+      <c r="B8" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-    </row>
-    <row r="9" spans="1:5" ht="30" customHeight="1">
-      <c r="A9" s="2"/>
-      <c r="B9" s="5" t="s">
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="1"/>
+      <c r="B9" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="7">
+      <c r="C9" s="6">
         <v>41001</v>
       </c>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-    </row>
-    <row r="10" spans="1:5" ht="30" customHeight="1">
-      <c r="A10" s="2"/>
-      <c r="B10" s="5" t="s">
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="1"/>
+      <c r="B10" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-    </row>
-    <row r="11" spans="1:5" ht="30" customHeight="1">
-      <c r="A11" s="2"/>
-      <c r="B11" s="5" t="s">
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+    </row>
+    <row r="11" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="1"/>
+      <c r="B11" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-    </row>
-    <row r="12" spans="1:5" ht="30" customHeight="1">
-      <c r="A12" s="2"/>
-      <c r="B12" s="5" t="s">
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+    </row>
+    <row r="12" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="1"/>
+      <c r="B12" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -960,1481 +958,1481 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="8"/>
-    <col min="2" max="3" width="10.83203125" style="9"/>
-    <col min="4" max="5" width="10.83203125" style="10"/>
-    <col min="6" max="6" width="10.83203125" style="8"/>
-    <col min="7" max="9" width="10.83203125" style="10"/>
-    <col min="10" max="10" width="10.83203125" style="8"/>
-    <col min="11" max="1025" width="10.83203125" style="10"/>
+    <col min="1" max="1" width="10.85546875" style="7"/>
+    <col min="2" max="3" width="10.85546875" style="8"/>
+    <col min="4" max="5" width="10.85546875" style="9"/>
+    <col min="6" max="6" width="10.85546875" style="7"/>
+    <col min="7" max="9" width="10.85546875" style="9"/>
+    <col min="10" max="10" width="10.85546875" style="7"/>
+    <col min="11" max="1025" width="10.85546875" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="10" customFormat="1" ht="56">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:9" s="9" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="H1" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="7" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="10" customFormat="1" ht="56">
-      <c r="A2" s="8">
+    <row r="2" spans="1:9" s="9" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A2" s="7">
         <v>1</v>
       </c>
-      <c r="B2" s="9">
+      <c r="B2" s="8">
         <v>41001</v>
       </c>
-      <c r="C2" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" s="10" t="s">
+      <c r="C2" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="9">
+      <c r="F2" s="8">
         <v>41003</v>
       </c>
-      <c r="H2" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="I2" s="8" t="s">
+      <c r="H2" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" s="7" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:9" s="10" customFormat="1" ht="70">
-      <c r="A3" s="8">
+    <row r="3" spans="1:9" s="9" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A3" s="7">
         <v>2</v>
       </c>
-      <c r="B3" s="9">
+      <c r="B3" s="8">
         <v>41001</v>
       </c>
-      <c r="C3" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="10" t="s">
+      <c r="C3" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="F3" s="9">
+      <c r="F3" s="8">
         <v>41057</v>
       </c>
-      <c r="H3" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="I3" s="8" t="s">
+      <c r="H3" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="I3" s="7" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:9" s="10" customFormat="1" ht="112">
-      <c r="A4" s="8">
+    <row r="4" spans="1:9" s="9" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+      <c r="A4" s="7">
         <v>3</v>
       </c>
-      <c r="B4" s="9">
+      <c r="B4" s="8">
         <v>41001</v>
       </c>
-      <c r="C4" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" s="10" t="s">
+      <c r="C4" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="F4" s="9">
+      <c r="F4" s="8">
         <v>41003</v>
       </c>
-      <c r="H4" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="I4" s="8" t="s">
+      <c r="H4" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="I4" s="7" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:9" s="10" customFormat="1" ht="126">
-      <c r="A5" s="8">
+    <row r="5" spans="1:9" s="9" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+      <c r="A5" s="7">
         <v>4</v>
       </c>
-      <c r="B5" s="9">
+      <c r="B5" s="8">
         <v>41001</v>
       </c>
-      <c r="C5" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="10" t="s">
+      <c r="C5" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="E5" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="F5" s="9">
+      <c r="F5" s="8">
         <v>41019</v>
       </c>
-      <c r="H5" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="I5" s="8" t="s">
+      <c r="H5" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="I5" s="7" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:9" s="10" customFormat="1" ht="28">
-      <c r="A6" s="8">
+    <row r="6" spans="1:9" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="7">
         <v>5</v>
       </c>
-      <c r="B6" s="9">
+      <c r="B6" s="8">
         <v>41001</v>
       </c>
-      <c r="C6" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" s="10" t="s">
+      <c r="C6" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="E6" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="F6" s="9">
+      <c r="F6" s="8">
         <v>41009</v>
       </c>
-      <c r="H6" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="I6" s="8" t="s">
+      <c r="H6" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="I6" s="7" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:9" s="10" customFormat="1" ht="42">
-      <c r="A7" s="8">
+    <row r="7" spans="1:9" s="9" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7" s="7">
         <v>6</v>
       </c>
-      <c r="B7" s="9">
+      <c r="B7" s="8">
         <v>41001</v>
       </c>
-      <c r="C7" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" s="10" t="s">
+      <c r="C7" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="E7" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="F7" s="9">
+      <c r="F7" s="8">
         <v>41003</v>
       </c>
-      <c r="H7" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="I7" s="8" t="s">
+      <c r="H7" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="I7" s="7" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:9" s="10" customFormat="1" ht="70">
-      <c r="A8" s="8">
+    <row r="8" spans="1:9" s="9" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A8" s="7">
         <v>7</v>
       </c>
-      <c r="B8" s="9">
+      <c r="B8" s="8">
         <v>41001</v>
       </c>
-      <c r="C8" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" s="10" t="s">
+      <c r="C8" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="E8" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="F8" s="9">
+      <c r="F8" s="8">
         <v>41003</v>
       </c>
-      <c r="H8" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="I8" s="8" t="s">
+      <c r="H8" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="I8" s="7" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:9" s="10" customFormat="1" ht="56">
-      <c r="A9" s="8">
+    <row r="9" spans="1:9" s="9" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A9" s="7">
         <v>8</v>
       </c>
-      <c r="B9" s="9">
+      <c r="B9" s="8">
         <v>41001</v>
       </c>
-      <c r="C9" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9" s="10" t="s">
+      <c r="C9" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="E9" s="10" t="s">
+      <c r="E9" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="F9" s="9">
+      <c r="F9" s="8">
         <v>41003</v>
       </c>
-      <c r="H9" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="I9" s="8" t="s">
+      <c r="H9" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="I9" s="7" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:9" s="10" customFormat="1" ht="84">
-      <c r="A10" s="8">
+    <row r="10" spans="1:9" s="9" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A10" s="7">
         <v>9</v>
       </c>
-      <c r="B10" s="9">
+      <c r="B10" s="8">
         <v>41009</v>
       </c>
-      <c r="C10" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" s="10" t="s">
+      <c r="C10" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="E10" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="F10" s="9">
+      <c r="F10" s="8">
         <v>41010</v>
       </c>
-      <c r="H10" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="I10" s="8" t="s">
+      <c r="H10" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="I10" s="7" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:9" s="10" customFormat="1" ht="84">
-      <c r="A11" s="8">
+    <row r="11" spans="1:9" s="9" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+      <c r="A11" s="7">
         <v>10</v>
       </c>
-      <c r="B11" s="9">
+      <c r="B11" s="8">
         <v>41009</v>
       </c>
-      <c r="C11" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D11" s="10" t="s">
+      <c r="C11" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="E11" s="10" t="s">
+      <c r="E11" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="F11" s="9">
+      <c r="F11" s="8">
         <v>41010</v>
       </c>
-      <c r="H11" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="I11" s="8" t="s">
+      <c r="H11" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="I11" s="7" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:9" s="10" customFormat="1" ht="56">
-      <c r="A12" s="8">
+    <row r="12" spans="1:9" s="9" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A12" s="7">
         <v>11</v>
       </c>
-      <c r="B12" s="9">
+      <c r="B12" s="8">
         <v>41009</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="C12" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="D12" s="10" t="s">
+      <c r="D12" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="E12" s="10" t="s">
+      <c r="E12" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="F12" s="9">
+      <c r="F12" s="8">
         <v>41000</v>
       </c>
-      <c r="H12" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="I12" s="8" t="s">
+      <c r="H12" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="I12" s="7" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:9" s="10" customFormat="1" ht="84">
-      <c r="A13" s="8">
+    <row r="13" spans="1:9" s="9" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A13" s="7">
         <v>12</v>
       </c>
-      <c r="B13" s="9">
+      <c r="B13" s="8">
         <v>41009</v>
       </c>
-      <c r="C13" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D13" s="10" t="s">
+      <c r="C13" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="E13" s="10" t="s">
+      <c r="E13" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="F13" s="9">
+      <c r="F13" s="8">
         <v>41010</v>
       </c>
-      <c r="H13" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="I13" s="8" t="s">
+      <c r="H13" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="I13" s="7" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:9" s="10" customFormat="1" ht="70">
-      <c r="A14" s="8">
+    <row r="14" spans="1:9" s="9" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A14" s="7">
         <v>13</v>
       </c>
-      <c r="B14" s="9">
+      <c r="B14" s="8">
         <v>41009</v>
       </c>
-      <c r="C14" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D14" s="10" t="s">
+      <c r="C14" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="E14" s="10" t="s">
+      <c r="E14" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="F14" s="9">
+      <c r="F14" s="8">
         <v>41010</v>
       </c>
-      <c r="H14" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="I14" s="8" t="s">
+      <c r="H14" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="I14" s="7" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:9" s="14" customFormat="1" ht="42">
-      <c r="A15" s="12">
+    <row r="15" spans="1:9" s="21" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A15" s="19">
         <v>14</v>
       </c>
-      <c r="B15" s="13">
+      <c r="B15" s="20">
         <v>41009</v>
       </c>
-      <c r="C15" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="D15" s="14" t="s">
+      <c r="C15" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="E15" s="14" t="s">
+      <c r="E15" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="F15" s="13">
+      <c r="F15" s="20">
         <v>41014</v>
       </c>
-      <c r="H15" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="I15" s="12" t="s">
+      <c r="H15" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="I15" s="19" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:9" s="10" customFormat="1" ht="70">
-      <c r="A16" s="8">
+    <row r="16" spans="1:9" s="9" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A16" s="7">
         <v>15</v>
       </c>
-      <c r="B16" s="9">
+      <c r="B16" s="8">
         <v>41009</v>
       </c>
-      <c r="C16" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D16" s="10" t="s">
+      <c r="C16" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="E16" s="10" t="s">
+      <c r="E16" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="F16" s="9">
+      <c r="F16" s="8">
         <v>41014</v>
       </c>
-      <c r="H16" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="I16" s="8" t="s">
+      <c r="H16" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="I16" s="7" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:10" s="10" customFormat="1" ht="112">
-      <c r="A17" s="12">
+    <row r="17" spans="1:10" s="21" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+      <c r="A17" s="19">
         <v>16</v>
       </c>
-      <c r="B17" s="13">
+      <c r="B17" s="20">
         <v>41001</v>
       </c>
-      <c r="C17" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="D17" s="14" t="s">
+      <c r="C17" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="E17" s="14" t="s">
+      <c r="E17" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="F17" s="13">
+      <c r="F17" s="20">
         <v>41014</v>
       </c>
-      <c r="G17" s="14"/>
-      <c r="H17" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="I17" s="12" t="s">
+      <c r="H17" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="I17" s="19" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:10" s="10" customFormat="1" ht="28">
-      <c r="A18" s="8">
+    <row r="18" spans="1:10" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A18" s="7">
         <v>17</v>
       </c>
-      <c r="B18" s="9">
+      <c r="B18" s="8">
         <v>41009</v>
       </c>
-      <c r="C18" s="9" t="s">
+      <c r="C18" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="D18" s="10" t="s">
+      <c r="D18" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="E18" s="10" t="s">
+      <c r="E18" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="F18" s="9">
+      <c r="F18" s="8">
         <v>41014</v>
       </c>
-      <c r="H18" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="I18" s="8" t="s">
+      <c r="H18" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="I18" s="7" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:10" s="10" customFormat="1" ht="28">
-      <c r="A19" s="8">
-        <v>18</v>
-      </c>
-      <c r="B19" s="9">
+    <row r="19" spans="1:10" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A19" s="7">
+        <v>18</v>
+      </c>
+      <c r="B19" s="8">
         <v>41009</v>
       </c>
-      <c r="C19" s="9" t="s">
+      <c r="C19" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="D19" s="10" t="s">
+      <c r="D19" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="E19" s="10" t="s">
+      <c r="E19" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="F19" s="9">
+      <c r="F19" s="8">
         <v>41028</v>
       </c>
-      <c r="H19" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="I19" s="8" t="s">
+      <c r="H19" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="I19" s="7" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:10" s="10" customFormat="1" ht="28">
-      <c r="A20" s="8">
+    <row r="20" spans="1:10" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" s="7">
         <v>19</v>
       </c>
-      <c r="B20" s="9">
+      <c r="B20" s="8">
         <v>41009</v>
       </c>
-      <c r="C20" s="9" t="s">
+      <c r="C20" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="D20" s="10" t="s">
+      <c r="D20" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="E20" s="10" t="s">
+      <c r="E20" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="F20" s="9">
+      <c r="F20" s="8">
         <v>41042</v>
       </c>
-      <c r="H20" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="I20" s="8" t="s">
+      <c r="H20" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="I20" s="7" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:10" s="10" customFormat="1" ht="28">
-      <c r="A21" s="8">
+    <row r="21" spans="1:10" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A21" s="7">
         <v>20</v>
       </c>
-      <c r="B21" s="9">
+      <c r="B21" s="8">
         <v>41009</v>
       </c>
-      <c r="C21" s="9" t="s">
+      <c r="C21" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="D21" s="10" t="s">
+      <c r="D21" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="E21" s="10" t="s">
+      <c r="E21" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="F21" s="9">
+      <c r="F21" s="8">
         <v>41056</v>
       </c>
-      <c r="H21" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="I21" s="8" t="s">
+      <c r="H21" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="I21" s="7" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:10" s="10" customFormat="1" ht="56">
-      <c r="A22" s="8">
-        <v>21</v>
-      </c>
-      <c r="B22" s="9">
+    <row r="22" spans="1:10" s="9" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A22" s="7">
+        <v>21</v>
+      </c>
+      <c r="B22" s="8">
         <v>41009</v>
       </c>
-      <c r="C22" s="9" t="s">
+      <c r="C22" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="D22" s="10" t="s">
+      <c r="D22" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="E22" s="10" t="s">
+      <c r="E22" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="F22" s="9">
+      <c r="F22" s="8">
         <v>41063</v>
       </c>
-      <c r="H22" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="I22" s="8" t="s">
+      <c r="H22" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="I22" s="7" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:10" s="10" customFormat="1" ht="56">
-      <c r="A23" s="8">
+    <row r="23" spans="1:10" s="9" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A23" s="7">
         <v>22</v>
       </c>
-      <c r="B23" s="9">
+      <c r="B23" s="8">
         <v>41009</v>
       </c>
-      <c r="C23" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D23" s="10" t="s">
+      <c r="C23" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D23" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="E23" s="10" t="s">
+      <c r="E23" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="F23" s="9">
+      <c r="F23" s="8">
         <v>41063</v>
       </c>
-      <c r="H23" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="I23" s="8" t="s">
+      <c r="H23" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="I23" s="7" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:10" s="10" customFormat="1" ht="70">
-      <c r="A24" s="15">
+    <row r="24" spans="1:10" s="9" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A24" s="11">
         <v>23</v>
       </c>
-      <c r="B24" s="9">
+      <c r="B24" s="8">
         <v>41009</v>
       </c>
-      <c r="C24" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="D24" s="17" t="s">
+      <c r="C24" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D24" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="E24" s="17" t="s">
+      <c r="E24" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="F24" s="9">
+      <c r="F24" s="8">
         <v>41011</v>
       </c>
-      <c r="G24" s="17"/>
-      <c r="H24" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="I24" s="15" t="s">
+      <c r="G24" s="13"/>
+      <c r="H24" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="I24" s="11" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:10" s="10" customFormat="1" ht="84">
-      <c r="A25" s="8">
+    <row r="25" spans="1:10" s="9" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A25" s="7">
         <v>24</v>
       </c>
-      <c r="B25" s="9">
+      <c r="B25" s="8">
         <v>41012</v>
       </c>
-      <c r="C25" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="D25" s="10" t="s">
+      <c r="C25" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D25" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="E25" s="17" t="s">
+      <c r="E25" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="F25" s="9">
+      <c r="F25" s="8">
         <v>41012</v>
       </c>
-      <c r="G25" s="17"/>
-      <c r="H25" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="I25" s="15" t="s">
+      <c r="G25" s="13"/>
+      <c r="H25" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="I25" s="11" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:10" s="10" customFormat="1" ht="56">
-      <c r="A26" s="8">
+    <row r="26" spans="1:10" s="9" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A26" s="7">
         <v>25</v>
       </c>
-      <c r="B26" s="9">
+      <c r="B26" s="8">
         <v>41012</v>
       </c>
-      <c r="C26" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="D26" s="17" t="s">
+      <c r="C26" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D26" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="E26" s="17" t="s">
+      <c r="E26" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="F26" s="9">
+      <c r="F26" s="8">
         <v>41014</v>
       </c>
-      <c r="G26" s="17"/>
-      <c r="H26" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="I26" s="15" t="s">
+      <c r="G26" s="13"/>
+      <c r="H26" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="I26" s="11" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="1:10" s="10" customFormat="1" ht="84">
-      <c r="A27" s="8">
+    <row r="27" spans="1:10" s="9" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A27" s="7">
         <v>26</v>
       </c>
-      <c r="B27" s="9">
+      <c r="B27" s="8">
         <v>41014</v>
       </c>
-      <c r="C27" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="D27" s="10" t="s">
+      <c r="C27" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D27" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="E27" s="17" t="s">
+      <c r="E27" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="F27" s="9">
+      <c r="F27" s="8">
         <v>41015</v>
       </c>
-      <c r="G27" s="17"/>
-      <c r="H27" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="I27" s="15" t="s">
+      <c r="G27" s="13"/>
+      <c r="H27" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="I27" s="11" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="28" spans="1:10" s="10" customFormat="1" ht="84">
-      <c r="A28" s="8">
+    <row r="28" spans="1:10" s="9" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A28" s="7">
         <v>27</v>
       </c>
-      <c r="B28" s="9">
+      <c r="B28" s="8">
         <v>41015</v>
       </c>
-      <c r="C28" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="D28" s="10" t="s">
+      <c r="C28" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D28" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="E28" s="17" t="s">
+      <c r="E28" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="F28" s="9">
+      <c r="F28" s="8">
         <v>41016</v>
       </c>
-      <c r="G28" s="17"/>
-      <c r="H28" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="I28" s="15" t="s">
+      <c r="G28" s="13"/>
+      <c r="H28" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="I28" s="11" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="29" spans="1:10" s="10" customFormat="1" ht="84">
-      <c r="A29" s="8">
+    <row r="29" spans="1:10" s="9" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A29" s="7">
         <v>28</v>
       </c>
-      <c r="B29" s="9">
+      <c r="B29" s="8">
         <v>41017</v>
       </c>
-      <c r="C29" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="D29" s="10" t="s">
+      <c r="C29" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D29" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="E29" s="17" t="s">
+      <c r="E29" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="F29" s="9">
+      <c r="F29" s="8">
         <v>41018</v>
       </c>
-      <c r="G29" s="17"/>
-      <c r="H29" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="I29" s="15" t="s">
+      <c r="G29" s="13"/>
+      <c r="H29" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="I29" s="11" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="30" spans="1:10" s="10" customFormat="1" ht="42">
-      <c r="A30" s="8">
+    <row r="30" spans="1:10" s="9" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A30" s="7">
         <v>29</v>
       </c>
-      <c r="B30" s="9">
+      <c r="B30" s="8">
         <v>41017</v>
       </c>
-      <c r="C30" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="D30" s="17" t="s">
+      <c r="C30" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D30" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="E30" s="17" t="s">
+      <c r="E30" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="F30" s="9">
+      <c r="F30" s="8">
         <v>41018</v>
       </c>
-      <c r="G30" s="17"/>
-      <c r="H30" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="I30" s="15" t="s">
+      <c r="G30" s="13"/>
+      <c r="H30" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="I30" s="11" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="14">
-      <c r="A31" s="8">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" s="7">
         <v>30</v>
       </c>
-      <c r="C31" s="16"/>
-      <c r="D31" s="17"/>
-      <c r="E31" s="17"/>
-      <c r="F31" s="9"/>
-      <c r="G31" s="17"/>
-      <c r="H31" s="17"/>
-      <c r="I31" s="15"/>
-      <c r="J31" s="10"/>
-    </row>
-    <row r="32" spans="1:10" s="10" customFormat="1" ht="42">
-      <c r="A32" s="8">
+      <c r="C31" s="12"/>
+      <c r="D31" s="13"/>
+      <c r="E31" s="13"/>
+      <c r="F31" s="8"/>
+      <c r="G31" s="13"/>
+      <c r="H31" s="13"/>
+      <c r="I31" s="11"/>
+      <c r="J31" s="9"/>
+    </row>
+    <row r="32" spans="1:10" s="9" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A32" s="7">
         <v>31</v>
       </c>
-      <c r="B32" s="9">
+      <c r="B32" s="8">
         <v>41017</v>
       </c>
-      <c r="C32" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="D32" s="10" t="s">
+      <c r="C32" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D32" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="E32" s="10" t="s">
+      <c r="E32" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="F32" s="9">
+      <c r="F32" s="8">
         <v>41022</v>
       </c>
-      <c r="H32" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="I32" s="8" t="s">
+      <c r="H32" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="I32" s="7" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="1:10" s="10" customFormat="1" ht="56">
-      <c r="A33" s="15">
+    <row r="33" spans="1:10" s="9" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A33" s="11">
         <v>32</v>
       </c>
-      <c r="B33" s="9">
+      <c r="B33" s="8">
         <v>41017</v>
       </c>
-      <c r="C33" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D33" s="10" t="s">
+      <c r="C33" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D33" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="E33" s="10" t="s">
+      <c r="E33" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="F33" s="9">
+      <c r="F33" s="8">
         <v>41022</v>
       </c>
-      <c r="H33" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="I33" s="8" t="s">
+      <c r="H33" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="I33" s="7" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="34" spans="1:10" s="10" customFormat="1" ht="28">
-      <c r="A34" s="8">
+    <row r="34" spans="1:10" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A34" s="7">
         <v>33</v>
       </c>
-      <c r="B34" s="9">
+      <c r="B34" s="8">
         <v>41017</v>
       </c>
-      <c r="C34" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D34" s="10" t="s">
+      <c r="C34" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D34" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="E34" s="10" t="s">
+      <c r="E34" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="F34" s="9">
+      <c r="F34" s="8">
         <v>41018</v>
       </c>
-      <c r="H34" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="I34" s="8" t="s">
+      <c r="H34" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="I34" s="7" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="35" spans="1:10" s="10" customFormat="1" ht="42">
-      <c r="A35" s="8">
+    <row r="35" spans="1:10" s="9" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A35" s="7">
         <v>34</v>
       </c>
-      <c r="B35" s="9">
+      <c r="B35" s="8">
         <v>41017</v>
       </c>
-      <c r="C35" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D35" s="10" t="s">
+      <c r="C35" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D35" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="E35" s="10" t="s">
+      <c r="E35" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="F35" s="9">
+      <c r="F35" s="8">
         <v>41019</v>
       </c>
-      <c r="H35" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="I35" s="8" t="s">
+      <c r="H35" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="I35" s="7" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="36" spans="1:10" s="10" customFormat="1" ht="70">
-      <c r="A36" s="8">
+    <row r="36" spans="1:10" s="9" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+      <c r="A36" s="7">
         <v>35</v>
       </c>
-      <c r="B36" s="9">
+      <c r="B36" s="8">
         <v>41017</v>
       </c>
-      <c r="C36" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D36" s="10" t="s">
+      <c r="C36" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D36" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="E36" s="10" t="s">
+      <c r="E36" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="F36" s="9"/>
-      <c r="H36" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="I36" s="8" t="s">
+      <c r="F36" s="8"/>
+      <c r="H36" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="I36" s="7" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="37" spans="1:10" s="10" customFormat="1" ht="42">
-      <c r="A37" s="8">
+    <row r="37" spans="1:10" s="9" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A37" s="7">
         <v>36</v>
       </c>
-      <c r="B37" s="9">
+      <c r="B37" s="8">
         <v>41017</v>
       </c>
-      <c r="C37" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D37" s="10" t="s">
+      <c r="C37" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D37" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="E37" s="10" t="s">
+      <c r="E37" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="F37" s="9"/>
-      <c r="H37" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="I37" s="8" t="s">
+      <c r="F37" s="8"/>
+      <c r="H37" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="I37" s="7" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="38" spans="1:10" s="10" customFormat="1" ht="140">
-      <c r="A38" s="8">
+    <row r="38" spans="1:10" s="9" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+      <c r="A38" s="7">
         <v>37</v>
       </c>
-      <c r="B38" s="9">
+      <c r="B38" s="8">
         <v>41017</v>
       </c>
-      <c r="C38" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D38" s="10" t="s">
+      <c r="C38" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D38" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="E38" s="10" t="s">
+      <c r="E38" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="F38" s="9"/>
-      <c r="H38" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="I38" s="8" t="s">
+      <c r="F38" s="8"/>
+      <c r="H38" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="I38" s="7" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="39" spans="1:10" s="10" customFormat="1" ht="42">
-      <c r="A39" s="8">
+    <row r="39" spans="1:10" s="9" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A39" s="7">
         <v>38</v>
       </c>
-      <c r="B39" s="9">
+      <c r="B39" s="8">
         <v>41017</v>
       </c>
-      <c r="C39" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D39" s="10" t="s">
+      <c r="C39" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D39" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="E39" s="10" t="s">
+      <c r="E39" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="F39" s="9"/>
-      <c r="H39" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="I39" s="8" t="s">
+      <c r="F39" s="8"/>
+      <c r="H39" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="I39" s="7" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="40" spans="1:10" s="10" customFormat="1" ht="112">
-      <c r="A40" s="8">
+    <row r="40" spans="1:10" s="9" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+      <c r="A40" s="7">
         <v>39</v>
       </c>
-      <c r="B40" s="9">
+      <c r="B40" s="8">
         <v>41017</v>
       </c>
-      <c r="C40" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D40" s="10" t="s">
+      <c r="C40" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D40" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="E40" s="10" t="s">
+      <c r="E40" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="F40" s="9"/>
-      <c r="H40" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="I40" s="8" t="s">
+      <c r="F40" s="8"/>
+      <c r="H40" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="I40" s="7" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="41" spans="1:10" s="10" customFormat="1" ht="98">
-      <c r="A41" s="8">
+    <row r="41" spans="1:10" s="9" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+      <c r="A41" s="7">
         <v>40</v>
       </c>
-      <c r="B41" s="9">
+      <c r="B41" s="8">
         <v>41017</v>
       </c>
-      <c r="C41" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D41" s="10" t="s">
+      <c r="C41" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D41" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="E41" s="10" t="s">
+      <c r="E41" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="F41" s="9"/>
-      <c r="H41" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="I41" s="8" t="s">
+      <c r="F41" s="8"/>
+      <c r="H41" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="I41" s="7" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="42" spans="1:10" s="10" customFormat="1" ht="42">
-      <c r="A42" s="8">
+    <row r="42" spans="1:10" s="9" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A42" s="7">
         <v>41</v>
       </c>
-      <c r="B42" s="9">
+      <c r="B42" s="8">
         <v>41018</v>
       </c>
-      <c r="C42" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D42" s="10" t="s">
+      <c r="C42" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D42" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="E42" s="10" t="s">
+      <c r="E42" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="F42" s="9"/>
-      <c r="H42" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="I42" s="8" t="s">
+      <c r="F42" s="8"/>
+      <c r="H42" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="I42" s="7" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="43" spans="1:10" s="10" customFormat="1" ht="84">
-      <c r="A43" s="8">
+    <row r="43" spans="1:10" s="9" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A43" s="7">
         <v>42</v>
       </c>
-      <c r="B43" s="9">
+      <c r="B43" s="8">
         <v>41028</v>
       </c>
-      <c r="C43" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D43" s="10" t="s">
+      <c r="C43" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D43" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="E43" s="10" t="s">
+      <c r="E43" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="F43" s="9"/>
-      <c r="H43" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="I43" s="8" t="s">
+      <c r="F43" s="8"/>
+      <c r="H43" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="I43" s="7" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="44" spans="1:10" s="10" customFormat="1" ht="70">
-      <c r="A44" s="15">
+    <row r="44" spans="1:10" s="9" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+      <c r="A44" s="11">
         <v>43</v>
       </c>
-      <c r="B44" s="9">
+      <c r="B44" s="8">
         <v>41028</v>
       </c>
-      <c r="C44" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D44" s="10" t="s">
+      <c r="C44" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D44" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="E44" s="10" t="s">
+      <c r="E44" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="F44" s="9"/>
-      <c r="H44" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="I44" s="8" t="s">
+      <c r="F44" s="8"/>
+      <c r="H44" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="I44" s="7" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="45" spans="1:10" s="10" customFormat="1" ht="70">
-      <c r="A45" s="8">
+    <row r="45" spans="1:10" s="9" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+      <c r="A45" s="7">
         <v>44</v>
       </c>
-      <c r="B45" s="9">
+      <c r="B45" s="8">
         <v>41028</v>
       </c>
-      <c r="C45" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D45" s="10" t="s">
+      <c r="C45" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D45" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="E45" s="10" t="s">
+      <c r="E45" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="F45" s="9"/>
-      <c r="H45" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="I45" s="8" t="s">
+      <c r="F45" s="8"/>
+      <c r="H45" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="I45" s="7" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="46" spans="1:10" ht="14">
-      <c r="F46" s="9"/>
-      <c r="I46" s="8"/>
-      <c r="J46" s="10"/>
-    </row>
-    <row r="47" spans="1:10" ht="14">
-      <c r="F47" s="9"/>
-      <c r="I47" s="8"/>
-      <c r="J47" s="10"/>
-    </row>
-    <row r="48" spans="1:10" ht="14">
-      <c r="F48" s="9"/>
-      <c r="I48" s="8"/>
-      <c r="J48" s="10"/>
-    </row>
-    <row r="49" spans="1:10" ht="14">
-      <c r="F49" s="9"/>
-      <c r="I49" s="8"/>
-      <c r="J49" s="10"/>
-    </row>
-    <row r="50" spans="1:10" ht="14">
-      <c r="F50" s="9"/>
-      <c r="I50" s="8"/>
-      <c r="J50" s="10"/>
-    </row>
-    <row r="51" spans="1:10" ht="14">
-      <c r="B51" s="18"/>
-      <c r="C51" s="19"/>
-      <c r="D51" s="20"/>
-      <c r="E51" s="20"/>
-      <c r="F51" s="20"/>
-      <c r="G51" s="20"/>
-      <c r="H51" s="20"/>
-      <c r="I51" s="21"/>
-      <c r="J51" s="10"/>
-    </row>
-    <row r="52" spans="1:10" ht="14">
-      <c r="B52" s="18"/>
-      <c r="C52" s="19"/>
-      <c r="D52" s="20"/>
-      <c r="E52" s="20"/>
-      <c r="F52" s="20"/>
-      <c r="G52" s="20"/>
-      <c r="H52" s="20"/>
-      <c r="I52" s="21"/>
-      <c r="J52" s="10"/>
-    </row>
-    <row r="53" spans="1:10" ht="14">
-      <c r="B53" s="18"/>
-      <c r="C53" s="19"/>
-      <c r="D53" s="20"/>
-      <c r="E53" s="20"/>
-      <c r="F53" s="20"/>
-      <c r="G53" s="20"/>
-      <c r="H53" s="20"/>
-      <c r="I53" s="21"/>
-      <c r="J53" s="10"/>
-    </row>
-    <row r="54" spans="1:10" s="10" customFormat="1" ht="14">
-      <c r="A54" s="15"/>
-      <c r="B54" s="18"/>
-      <c r="C54" s="19"/>
-      <c r="D54" s="20"/>
-      <c r="E54" s="20"/>
-      <c r="F54" s="20"/>
-      <c r="G54" s="20"/>
-      <c r="H54" s="20"/>
-      <c r="I54" s="21"/>
-    </row>
-    <row r="55" spans="1:10" ht="14">
-      <c r="B55" s="18"/>
-      <c r="C55" s="19"/>
-      <c r="D55" s="20"/>
-      <c r="E55" s="20"/>
-      <c r="F55" s="20"/>
-      <c r="G55" s="20"/>
-      <c r="H55" s="20"/>
-      <c r="I55" s="21"/>
-      <c r="J55" s="10"/>
-    </row>
-    <row r="56" spans="1:10" ht="14">
-      <c r="B56" s="18"/>
-      <c r="C56" s="19"/>
-      <c r="D56" s="20"/>
-      <c r="E56" s="20"/>
-      <c r="F56" s="20"/>
-      <c r="G56" s="20"/>
-      <c r="H56" s="20"/>
-      <c r="I56" s="21"/>
-      <c r="J56" s="10"/>
-    </row>
-    <row r="57" spans="1:10" ht="14">
-      <c r="B57" s="18"/>
-      <c r="C57" s="19"/>
-      <c r="D57" s="20"/>
-      <c r="J57" s="10"/>
-    </row>
-    <row r="58" spans="1:10" ht="14">
-      <c r="F58" s="9"/>
-      <c r="I58" s="8"/>
-      <c r="J58" s="10"/>
-    </row>
-    <row r="59" spans="1:10" ht="14">
-      <c r="F59" s="9"/>
-      <c r="I59" s="8"/>
-      <c r="J59" s="10"/>
-    </row>
-    <row r="60" spans="1:10" ht="14">
-      <c r="F60" s="9"/>
-      <c r="I60" s="8"/>
-      <c r="J60" s="10"/>
-    </row>
-    <row r="61" spans="1:10" ht="14">
-      <c r="F61" s="9"/>
-      <c r="I61" s="8"/>
-      <c r="J61" s="10"/>
-    </row>
-    <row r="62" spans="1:10" ht="14">
-      <c r="F62" s="9"/>
-      <c r="I62" s="8"/>
-      <c r="J62" s="10"/>
-    </row>
-    <row r="63" spans="1:10" ht="14">
-      <c r="F63" s="9"/>
-      <c r="I63" s="8"/>
-      <c r="J63" s="10"/>
-    </row>
-    <row r="64" spans="1:10" ht="14">
-      <c r="F64" s="9"/>
-      <c r="I64" s="8"/>
-      <c r="J64" s="10"/>
-    </row>
-    <row r="65" spans="1:10" ht="14">
-      <c r="F65" s="9"/>
-      <c r="I65" s="8"/>
-      <c r="J65" s="10"/>
-    </row>
-    <row r="66" spans="1:10" ht="14">
-      <c r="F66" s="9"/>
-      <c r="I66" s="8"/>
-      <c r="J66" s="10"/>
-    </row>
-    <row r="67" spans="1:10" ht="14">
-      <c r="F67" s="9"/>
-      <c r="I67" s="8"/>
-      <c r="J67" s="10"/>
-    </row>
-    <row r="68" spans="1:10" ht="14">
-      <c r="F68" s="9"/>
-      <c r="I68" s="8"/>
-      <c r="J68" s="10"/>
-    </row>
-    <row r="69" spans="1:10" ht="14">
-      <c r="F69" s="9"/>
-      <c r="I69" s="8"/>
-      <c r="J69" s="10"/>
-    </row>
-    <row r="70" spans="1:10" ht="14">
-      <c r="A70" s="15"/>
-      <c r="F70" s="9"/>
-      <c r="I70" s="8"/>
-      <c r="J70" s="10"/>
-    </row>
-    <row r="71" spans="1:10" ht="14">
-      <c r="F71" s="9"/>
-      <c r="I71" s="8"/>
-      <c r="J71" s="10"/>
-    </row>
-    <row r="72" spans="1:10" ht="14">
-      <c r="F72" s="9"/>
-      <c r="I72" s="8"/>
-      <c r="J72" s="10"/>
-    </row>
-    <row r="73" spans="1:10" ht="14">
-      <c r="F73" s="9"/>
-      <c r="I73" s="8"/>
-      <c r="J73" s="10"/>
-    </row>
-    <row r="74" spans="1:10" ht="14">
-      <c r="F74" s="9"/>
-      <c r="I74" s="8"/>
-      <c r="J74" s="10"/>
-    </row>
-    <row r="75" spans="1:10" ht="14">
-      <c r="F75" s="9"/>
-      <c r="I75" s="8"/>
-      <c r="J75" s="10"/>
-    </row>
-    <row r="76" spans="1:10" ht="14">
-      <c r="F76" s="9"/>
-      <c r="I76" s="8"/>
-      <c r="J76" s="10"/>
-    </row>
-    <row r="77" spans="1:10" ht="14">
-      <c r="F77" s="9"/>
-      <c r="I77" s="8"/>
-      <c r="J77" s="10"/>
-    </row>
-    <row r="78" spans="1:10" ht="14">
-      <c r="A78" s="8">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F46" s="8"/>
+      <c r="I46" s="7"/>
+      <c r="J46" s="9"/>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F47" s="8"/>
+      <c r="I47" s="7"/>
+      <c r="J47" s="9"/>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F48" s="8"/>
+      <c r="I48" s="7"/>
+      <c r="J48" s="9"/>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F49" s="8"/>
+      <c r="I49" s="7"/>
+      <c r="J49" s="9"/>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F50" s="8"/>
+      <c r="I50" s="7"/>
+      <c r="J50" s="9"/>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B51" s="14"/>
+      <c r="C51" s="15"/>
+      <c r="D51" s="16"/>
+      <c r="E51" s="16"/>
+      <c r="F51" s="16"/>
+      <c r="G51" s="16"/>
+      <c r="H51" s="16"/>
+      <c r="I51" s="17"/>
+      <c r="J51" s="9"/>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B52" s="14"/>
+      <c r="C52" s="15"/>
+      <c r="D52" s="16"/>
+      <c r="E52" s="16"/>
+      <c r="F52" s="16"/>
+      <c r="G52" s="16"/>
+      <c r="H52" s="16"/>
+      <c r="I52" s="17"/>
+      <c r="J52" s="9"/>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B53" s="14"/>
+      <c r="C53" s="15"/>
+      <c r="D53" s="16"/>
+      <c r="E53" s="16"/>
+      <c r="F53" s="16"/>
+      <c r="G53" s="16"/>
+      <c r="H53" s="16"/>
+      <c r="I53" s="17"/>
+      <c r="J53" s="9"/>
+    </row>
+    <row r="54" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="11"/>
+      <c r="B54" s="14"/>
+      <c r="C54" s="15"/>
+      <c r="D54" s="16"/>
+      <c r="E54" s="16"/>
+      <c r="F54" s="16"/>
+      <c r="G54" s="16"/>
+      <c r="H54" s="16"/>
+      <c r="I54" s="17"/>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B55" s="14"/>
+      <c r="C55" s="15"/>
+      <c r="D55" s="16"/>
+      <c r="E55" s="16"/>
+      <c r="F55" s="16"/>
+      <c r="G55" s="16"/>
+      <c r="H55" s="16"/>
+      <c r="I55" s="17"/>
+      <c r="J55" s="9"/>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B56" s="14"/>
+      <c r="C56" s="15"/>
+      <c r="D56" s="16"/>
+      <c r="E56" s="16"/>
+      <c r="F56" s="16"/>
+      <c r="G56" s="16"/>
+      <c r="H56" s="16"/>
+      <c r="I56" s="17"/>
+      <c r="J56" s="9"/>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B57" s="14"/>
+      <c r="C57" s="15"/>
+      <c r="D57" s="16"/>
+      <c r="J57" s="9"/>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F58" s="8"/>
+      <c r="I58" s="7"/>
+      <c r="J58" s="9"/>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F59" s="8"/>
+      <c r="I59" s="7"/>
+      <c r="J59" s="9"/>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F60" s="8"/>
+      <c r="I60" s="7"/>
+      <c r="J60" s="9"/>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F61" s="8"/>
+      <c r="I61" s="7"/>
+      <c r="J61" s="9"/>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F62" s="8"/>
+      <c r="I62" s="7"/>
+      <c r="J62" s="9"/>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F63" s="8"/>
+      <c r="I63" s="7"/>
+      <c r="J63" s="9"/>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F64" s="8"/>
+      <c r="I64" s="7"/>
+      <c r="J64" s="9"/>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F65" s="8"/>
+      <c r="I65" s="7"/>
+      <c r="J65" s="9"/>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F66" s="8"/>
+      <c r="I66" s="7"/>
+      <c r="J66" s="9"/>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F67" s="8"/>
+      <c r="I67" s="7"/>
+      <c r="J67" s="9"/>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F68" s="8"/>
+      <c r="I68" s="7"/>
+      <c r="J68" s="9"/>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F69" s="8"/>
+      <c r="I69" s="7"/>
+      <c r="J69" s="9"/>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A70" s="11"/>
+      <c r="F70" s="8"/>
+      <c r="I70" s="7"/>
+      <c r="J70" s="9"/>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F71" s="8"/>
+      <c r="I71" s="7"/>
+      <c r="J71" s="9"/>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F72" s="8"/>
+      <c r="I72" s="7"/>
+      <c r="J72" s="9"/>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F73" s="8"/>
+      <c r="I73" s="7"/>
+      <c r="J73" s="9"/>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F74" s="8"/>
+      <c r="I74" s="7"/>
+      <c r="J74" s="9"/>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F75" s="8"/>
+      <c r="I75" s="7"/>
+      <c r="J75" s="9"/>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F76" s="8"/>
+      <c r="I76" s="7"/>
+      <c r="J76" s="9"/>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F77" s="8"/>
+      <c r="I77" s="7"/>
+      <c r="J77" s="9"/>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A78" s="7">
         <v>70</v>
       </c>
-      <c r="F78" s="9"/>
-      <c r="I78" s="8"/>
-      <c r="J78" s="10"/>
-    </row>
-    <row r="79" spans="1:10" ht="14">
-      <c r="A79" s="8">
+      <c r="F78" s="8"/>
+      <c r="I78" s="7"/>
+      <c r="J78" s="9"/>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A79" s="7">
         <v>71</v>
       </c>
-      <c r="F79" s="9"/>
-      <c r="I79" s="8"/>
-      <c r="J79" s="10"/>
-    </row>
-    <row r="80" spans="1:10" ht="14">
-      <c r="A80" s="15">
+      <c r="F79" s="8"/>
+      <c r="I79" s="7"/>
+      <c r="J79" s="9"/>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A80" s="11">
         <v>72</v>
       </c>
-      <c r="F80" s="9"/>
-      <c r="I80" s="8"/>
-      <c r="J80" s="10"/>
-    </row>
-    <row r="81" spans="1:10" ht="14">
-      <c r="A81" s="8">
+      <c r="F80" s="8"/>
+      <c r="I80" s="7"/>
+      <c r="J80" s="9"/>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A81" s="7">
         <v>73</v>
       </c>
-      <c r="F81" s="9"/>
-      <c r="I81" s="8"/>
-      <c r="J81" s="10"/>
-    </row>
-    <row r="82" spans="1:10" ht="14">
-      <c r="A82" s="8">
+      <c r="F81" s="8"/>
+      <c r="I81" s="7"/>
+      <c r="J81" s="9"/>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A82" s="7">
         <v>74</v>
       </c>
-      <c r="F82" s="9"/>
-      <c r="I82" s="8"/>
-      <c r="J82" s="10"/>
-    </row>
-    <row r="83" spans="1:10" ht="14">
-      <c r="A83" s="8">
+      <c r="F82" s="8"/>
+      <c r="I82" s="7"/>
+      <c r="J82" s="9"/>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A83" s="7">
         <v>75</v>
       </c>
-      <c r="F83" s="9"/>
-      <c r="I83" s="8"/>
-      <c r="J83" s="10"/>
-    </row>
-    <row r="84" spans="1:10" ht="14">
-      <c r="A84" s="8">
+      <c r="F83" s="8"/>
+      <c r="I83" s="7"/>
+      <c r="J83" s="9"/>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A84" s="7">
         <v>76</v>
       </c>
-      <c r="F84" s="9"/>
-      <c r="I84" s="8"/>
-      <c r="J84" s="10"/>
-    </row>
-    <row r="85" spans="1:10" ht="14">
-      <c r="A85" s="8">
+      <c r="F84" s="8"/>
+      <c r="I84" s="7"/>
+      <c r="J84" s="9"/>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A85" s="7">
         <v>77</v>
       </c>
-      <c r="F85" s="9"/>
-      <c r="I85" s="8"/>
-      <c r="J85" s="10"/>
-    </row>
-    <row r="86" spans="1:10" ht="14">
-      <c r="A86" s="8">
+      <c r="F85" s="8"/>
+      <c r="I85" s="7"/>
+      <c r="J85" s="9"/>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A86" s="7">
         <v>78</v>
       </c>
-      <c r="F86" s="9"/>
-      <c r="I86" s="8"/>
-      <c r="J86" s="10"/>
-    </row>
-    <row r="87" spans="1:10" ht="14">
-      <c r="A87" s="8">
+      <c r="F86" s="8"/>
+      <c r="I86" s="7"/>
+      <c r="J86" s="9"/>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A87" s="7">
         <v>79</v>
       </c>
-      <c r="F87" s="9"/>
-      <c r="I87" s="8"/>
-      <c r="J87" s="10"/>
-    </row>
-    <row r="88" spans="1:10" ht="14">
-      <c r="A88" s="8">
+      <c r="F87" s="8"/>
+      <c r="I87" s="7"/>
+      <c r="J87" s="9"/>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A88" s="7">
         <v>80</v>
       </c>
-      <c r="F88" s="9"/>
-      <c r="I88" s="8"/>
-      <c r="J88" s="10"/>
-    </row>
-    <row r="89" spans="1:10" ht="14">
-      <c r="A89" s="8">
+      <c r="F88" s="8"/>
+      <c r="I88" s="7"/>
+      <c r="J88" s="9"/>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A89" s="7">
         <v>81</v>
       </c>
-      <c r="F89" s="9"/>
-      <c r="I89" s="8"/>
-      <c r="J89" s="10"/>
-    </row>
-    <row r="90" spans="1:10" ht="14">
-      <c r="A90" s="8">
+      <c r="F89" s="8"/>
+      <c r="I89" s="7"/>
+      <c r="J89" s="9"/>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A90" s="7">
         <v>82</v>
       </c>
-      <c r="F90" s="9"/>
-      <c r="I90" s="8"/>
-      <c r="J90" s="10"/>
-    </row>
-    <row r="91" spans="1:10" ht="14">
-      <c r="A91" s="8">
+      <c r="F90" s="8"/>
+      <c r="I90" s="7"/>
+      <c r="J90" s="9"/>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A91" s="7">
         <v>83</v>
       </c>
-      <c r="F91" s="9"/>
-      <c r="I91" s="8"/>
-      <c r="J91" s="10"/>
+      <c r="F91" s="8"/>
+      <c r="I91" s="7"/>
+      <c r="J91" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -2449,7 +2447,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <extLst>

</xml_diff>